<commit_message>
Add rule check null data import timetable
</commit_message>
<xml_diff>
--- a/Content/Uploads/ImportTKB/ThoiKhoaBieu_TieuChuan_Mau2.xlsx
+++ b/Content/Uploads/ImportTKB/ThoiKhoaBieu_TieuChuan_Mau2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\CAPSTONE2024-DOCX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B619C7-1563-4C97-833D-D1265BA6C3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96F4482-6CF9-4409-ABE6-69F24BD53C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="102">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -1253,10 +1253,10 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
+      <selection pane="bottomRight" activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1274,7 +1274,7 @@
     <col min="16" max="16" width="13.69921875" customWidth="1"/>
     <col min="17" max="17" width="23.59765625" customWidth="1"/>
     <col min="19" max="24" width="9.09765625" customWidth="1"/>
-    <col min="25" max="25" width="23.19921875" customWidth="1"/>
+    <col min="25" max="25" width="8" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="21.3984375" customWidth="1"/>
     <col min="27" max="27" width="21.59765625" customWidth="1"/>
     <col min="28" max="28" width="23.296875" customWidth="1"/>
@@ -1608,11 +1608,11 @@
       <c r="K4" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="L4" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>33</v>
+      <c r="L4" s="8">
+        <v>4</v>
+      </c>
+      <c r="M4" s="8">
+        <v>3</v>
       </c>
       <c r="N4" s="8" t="s">
         <v>70</v>
@@ -1647,8 +1647,8 @@
       <c r="X4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="Y4" s="8" t="s">
-        <v>69</v>
+      <c r="Y4" s="8">
+        <v>4</v>
       </c>
       <c r="Z4" s="8" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Add function view timetable
</commit_message>
<xml_diff>
--- a/Content/Uploads/ImportTKB/ThoiKhoaBieu_TieuChuan_Mau2.xlsx
+++ b/Content/Uploads/ImportTKB/ThoiKhoaBieu_TieuChuan_Mau2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\CAPSTONE2024-DOCX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96F4482-6CF9-4409-ABE6-69F24BD53C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E207135D-2203-4B1E-83D4-50136297286A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="101">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -293,9 +293,6 @@
   </si>
   <si>
     <t>CS3.F.12.05</t>
-  </si>
-  <si>
-    <t>2001100524</t>
   </si>
   <si>
     <t>Nguyễn Hồng Diên</t>
@@ -1253,10 +1250,10 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P3" sqref="P3"/>
+      <selection pane="bottomRight" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1269,7 +1266,8 @@
     <col min="6" max="6" width="10.8984375" customWidth="1"/>
     <col min="7" max="7" width="14.8984375" style="2" customWidth="1"/>
     <col min="8" max="8" width="8.8984375" customWidth="1"/>
-    <col min="12" max="13" width="9.09765625" customWidth="1"/>
+    <col min="12" max="12" width="9.09765625" customWidth="1"/>
+    <col min="13" max="13" width="8.69921875" customWidth="1"/>
     <col min="15" max="15" width="13.59765625" customWidth="1"/>
     <col min="16" max="16" width="13.69921875" customWidth="1"/>
     <col min="17" max="17" width="23.59765625" customWidth="1"/>
@@ -1295,7 +1293,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -1376,7 +1374,7 @@
         <v>28</v>
       </c>
       <c r="AE1" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AF1" s="4" t="s">
         <v>29</v>
@@ -1428,8 +1426,8 @@
       <c r="O2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="10" t="s">
-        <v>38</v>
+      <c r="P2" s="10">
+        <v>2001100524</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>43</v>
@@ -1812,7 +1810,9 @@
       <c r="O6" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="P6" s="11"/>
+      <c r="P6" s="11">
+        <v>2001100524</v>
+      </c>
       <c r="Q6" s="11" t="s">
         <v>43</v>
       </c>
@@ -1906,11 +1906,11 @@
       <c r="O7" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="8">
+        <v>2001100520</v>
+      </c>
+      <c r="Q7" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>62</v>
@@ -1958,13 +1958,13 @@
     </row>
     <row r="8" spans="1:32" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>32</v>
@@ -1976,7 +1976,7 @@
         <v>57</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>36</v>
@@ -2002,11 +2002,11 @@
       <c r="O8" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="P8" s="8" t="s">
+      <c r="P8" s="8">
+        <v>2001100520</v>
+      </c>
+      <c r="Q8" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="Q8" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>62</v>
@@ -2054,13 +2054,13 @@
     </row>
     <row r="9" spans="1:32" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>32</v>
@@ -2072,7 +2072,7 @@
         <v>57</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>36</v>
@@ -2087,13 +2087,13 @@
         <v>58</v>
       </c>
       <c r="L9" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="O9" s="8" t="s">
         <v>59</v>
@@ -2126,7 +2126,7 @@
         <v>65</v>
       </c>
       <c r="Y9" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Z9" s="8" t="s">
         <v>51</v>
@@ -2150,13 +2150,13 @@
     </row>
     <row r="10" spans="1:32" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>32</v>
@@ -2168,7 +2168,7 @@
         <v>34</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>36</v>
@@ -2195,10 +2195,10 @@
         <v>78</v>
       </c>
       <c r="P10" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q10" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="Q10" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="R10" s="8" t="s">
         <v>44</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="11" spans="1:32" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>32</v>
@@ -2264,7 +2264,7 @@
         <v>57</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>36</v>
@@ -2276,7 +2276,7 @@
         <v>38</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>50</v>
@@ -2291,10 +2291,10 @@
         <v>59</v>
       </c>
       <c r="P11" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q11" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="Q11" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="R11" s="8" t="s">
         <v>62</v>

</xml_diff>